<commit_message>
Mini Project III - II
</commit_message>
<xml_diff>
--- a/Datasets/World Energy Overview.xlsx
+++ b/Datasets/World Energy Overview.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KARTHIKEYA\Desktop\Mini Project\Datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E8904E06-B806-4BFE-B2A7-FE619B66691B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{016AE276-FC6C-4795-AC08-0C1B8FC25C92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{34052753-8B3E-4B28-BA45-BCDBACE22682}"/>
   </bookViews>
@@ -201,7 +201,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -381,6 +381,12 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -542,9 +548,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -902,8 +909,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23F96F86-A71F-48A1-889E-F7DFFC840B8F}">
   <dimension ref="A1:M600"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:K1048576"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -918,48 +925,50 @@
     <col min="8" max="8" width="23.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="33.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="26.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="31.21875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="31.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="33" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="30.21875" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>